<commit_message>
setup fixtures to match import file
</commit_message>
<xml_diff>
--- a/test/fixtures/files/product_keyword_information_test.xlsx
+++ b/test/fixtures/files/product_keyword_information_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,24 +15,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
-  <si>
-    <t>tuotenumero</t>
-  </si>
-  <si>
-    <t>Tuotteen väri</t>
-  </si>
-  <si>
-    <t>toiminto</t>
-  </si>
-  <si>
-    <t>A1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+  <si>
+    <t>Tuotenumero</t>
+  </si>
+  <si>
+    <t>Tuotteen materiaali</t>
+  </si>
+  <si>
+    <t>Poista</t>
+  </si>
+  <si>
+    <t>hammer123</t>
   </si>
   <si>
     <t>Punainen</t>
   </si>
   <si>
-    <t>Musta</t>
+    <t>ski1</t>
+  </si>
+  <si>
+    <t>Sininen</t>
+  </si>
+  <si>
+    <t>Aluminium</t>
   </si>
   <si>
     <t>X</t>
@@ -50,6 +56,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -131,15 +138,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.10714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -163,13 +173,21 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>6</v>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>